<commit_message>
Uploaded all localized strings to Contentful
</commit_message>
<xml_diff>
--- a/loca/Loca_Keys_Strings_DE_EN.xlsx
+++ b/loca/Loca_Keys_Strings_DE_EN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\Desktop\vintage-poker\loca\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B342B19B-8F63-47E2-BEAF-B1EBE35CC132}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD34E3A-8BBC-44DA-8D7C-C17AC109E28B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28733" yWindow="3840" windowWidth="16875" windowHeight="10635" xr2:uid="{94609645-BEC5-4C02-AAB5-847C7763F872}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="121">
   <si>
     <t>Key</t>
   </si>
@@ -171,15 +171,6 @@
     <t>cookiebanner-confirm_btn_txt</t>
   </si>
   <si>
-    <t>OK</t>
-  </si>
-  <si>
-    <t>Policy</t>
-  </si>
-  <si>
-    <t>Datenschutz</t>
-  </si>
-  <si>
     <t>This website uses cookies. If you continue to use the website, we assume your consent.</t>
   </si>
   <si>
@@ -388,13 +379,25 @@
     <t>Registration</t>
   </si>
   <si>
-    <t>Registrierung Abschließen</t>
-  </si>
-  <si>
     <t>Ich habe bereits einen Account</t>
   </si>
   <si>
     <t>Spielername</t>
+  </si>
+  <si>
+    <t>Confirm</t>
+  </si>
+  <si>
+    <t>Bestätigen</t>
+  </si>
+  <si>
+    <t>Info</t>
+  </si>
+  <si>
+    <t>Information</t>
+  </si>
+  <si>
+    <t>Registrierung abschließen</t>
   </si>
 </sst>
 </file>
@@ -438,10 +441,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -770,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBD24C1D-54A3-4D83-9E6C-EC9C7BE97A48}">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -793,498 +796,498 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="C18" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>64</v>
-      </c>
-      <c r="B17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B26" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>65</v>
-      </c>
-      <c r="B18" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
-        <v>56</v>
-      </c>
-      <c r="B25" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
+      <c r="B27" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B26" t="s">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C26" t="s">
+      <c r="B28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A32" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A33" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A34" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>70</v>
-      </c>
-      <c r="B27" t="s">
-        <v>73</v>
-      </c>
-      <c r="C27" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>74</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="C34" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A35" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A36" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A37" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C37" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A38" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A39" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A40" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A41" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A42" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B29" t="s">
-        <v>79</v>
-      </c>
-      <c r="C29" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>76</v>
-      </c>
-      <c r="B30" t="s">
-        <v>81</v>
-      </c>
-      <c r="C30" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
-        <v>77</v>
-      </c>
-      <c r="B31" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>85</v>
-      </c>
-      <c r="B32" t="s">
-        <v>86</v>
-      </c>
-      <c r="C32" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
-        <v>84</v>
-      </c>
-      <c r="B33" t="s">
-        <v>87</v>
-      </c>
-      <c r="C33" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
-        <v>91</v>
-      </c>
-      <c r="B34" t="s">
-        <v>93</v>
-      </c>
-      <c r="C34" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
-        <v>92</v>
-      </c>
-      <c r="B35" t="s">
-        <v>95</v>
-      </c>
-      <c r="C35" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
-        <v>97</v>
-      </c>
-      <c r="B36" t="s">
-        <v>16</v>
-      </c>
-      <c r="C36" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
-        <v>98</v>
-      </c>
-      <c r="B37" t="s">
-        <v>81</v>
-      </c>
-      <c r="C37" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
+      <c r="C42" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A43" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A44" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B38" t="s">
-        <v>102</v>
-      </c>
-      <c r="C38" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
-        <v>100</v>
-      </c>
-      <c r="B39" t="s">
-        <v>103</v>
-      </c>
-      <c r="C39" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
+      <c r="C44" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B40" t="s">
-        <v>105</v>
-      </c>
-      <c r="C40" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A45" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B41" t="s">
-        <v>116</v>
-      </c>
-      <c r="C41" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
-        <v>115</v>
-      </c>
-      <c r="B42" t="s">
-        <v>78</v>
-      </c>
-      <c r="C42" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
+      <c r="B45" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A46" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B43" t="s">
-        <v>81</v>
-      </c>
-      <c r="C43" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
+      <c r="B46" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B44" t="s">
-        <v>102</v>
-      </c>
-      <c r="C44" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
-        <v>111</v>
-      </c>
-      <c r="B45" t="s">
+      <c r="C46" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="C45" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
-        <v>112</v>
-      </c>
-      <c r="B46" t="s">
-        <v>113</v>
-      </c>
-      <c r="C46" t="s">
-        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added localized string for serviceworker modal
</commit_message>
<xml_diff>
--- a/loca/Loca_Keys_Strings_DE_EN.xlsx
+++ b/loca/Loca_Keys_Strings_DE_EN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\Desktop\vintage-poker\loca\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD34E3A-8BBC-44DA-8D7C-C17AC109E28B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0624B794-63B2-4D18-AFDD-626B03746A8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28733" yWindow="3840" windowWidth="16875" windowHeight="10635" xr2:uid="{94609645-BEC5-4C02-AAB5-847C7763F872}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="124">
   <si>
     <t>Key</t>
   </si>
@@ -398,6 +398,16 @@
   </si>
   <si>
     <t>Registrierung abschließen</t>
+  </si>
+  <si>
+    <t>service_worker-update_available</t>
+  </si>
+  <si>
+    <t>A new update is available. Click the button below to refresh the app and get the latest and greatest stuff!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Ein neues Update ist verfügbar. Klicken Sie auf die Schaltfläche unten, um die App zu aktualisieren und die neuesten und besten Inhalte zu erhalten!</t>
   </si>
 </sst>
 </file>
@@ -463,8 +473,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6C946B8B-E002-4E29-8858-D6BCF5F62F16}" name="Tabelle2" displayName="Tabelle2" ref="A1:C46" totalsRowShown="0">
-  <autoFilter ref="A1:C46" xr:uid="{57128861-3067-4F74-9528-2F4689EA718A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6C946B8B-E002-4E29-8858-D6BCF5F62F16}" name="Tabelle2" displayName="Tabelle2" ref="A1:C47" totalsRowShown="0">
+  <autoFilter ref="A1:C47" xr:uid="{57128861-3067-4F74-9528-2F4689EA718A}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{F4919082-BBD5-45D0-9C5B-DAEF1991A8AA}" name="Key"/>
     <tableColumn id="2" xr3:uid="{D5FECD6D-54D4-413E-86EE-CACF52D2DA63}" name="String EN"/>
@@ -771,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBD24C1D-54A3-4D83-9E6C-EC9C7BE97A48}">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1290,6 +1300,17 @@
         <v>114</v>
       </c>
     </row>
+    <row r="47" spans="1:3" ht="57" x14ac:dyDescent="0.45">
+      <c r="A47" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added localized strings for sw update-modal
</commit_message>
<xml_diff>
--- a/loca/Loca_Keys_Strings_DE_EN.xlsx
+++ b/loca/Loca_Keys_Strings_DE_EN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\Desktop\vintage-poker\loca\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0624B794-63B2-4D18-AFDD-626B03746A8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605AF17A-3932-4AF9-ACB9-BC3B4D6CDFAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28733" yWindow="3840" windowWidth="16875" windowHeight="10635" xr2:uid="{94609645-BEC5-4C02-AAB5-847C7763F872}"/>
+    <workbookView xWindow="-21300" yWindow="1972" windowWidth="21600" windowHeight="11535" xr2:uid="{94609645-BEC5-4C02-AAB5-847C7763F872}"/>
   </bookViews>
   <sheets>
     <sheet name="KeyValuePairs" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="130">
   <si>
     <t>Key</t>
   </si>
@@ -408,6 +408,24 @@
   <si>
     <t xml:space="preserve">
 Ein neues Update ist verfügbar. Klicken Sie auf die Schaltfläche unten, um die App zu aktualisieren und die neuesten und besten Inhalte zu erhalten!</t>
+  </si>
+  <si>
+    <t>service_worker-update_headline</t>
+  </si>
+  <si>
+    <t>service_worker-update_confirm_btn_txt</t>
+  </si>
+  <si>
+    <t>Update Available</t>
+  </si>
+  <si>
+    <t>Update verfügbar</t>
+  </si>
+  <si>
+    <t>Update Now &amp; Refresh</t>
+  </si>
+  <si>
+    <t>Update installieren</t>
   </si>
 </sst>
 </file>
@@ -473,8 +491,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6C946B8B-E002-4E29-8858-D6BCF5F62F16}" name="Tabelle2" displayName="Tabelle2" ref="A1:C47" totalsRowShown="0">
-  <autoFilter ref="A1:C47" xr:uid="{57128861-3067-4F74-9528-2F4689EA718A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6C946B8B-E002-4E29-8858-D6BCF5F62F16}" name="Tabelle2" displayName="Tabelle2" ref="A1:C49" totalsRowShown="0">
+  <autoFilter ref="A1:C49" xr:uid="{57128861-3067-4F74-9528-2F4689EA718A}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{F4919082-BBD5-45D0-9C5B-DAEF1991A8AA}" name="Key"/>
     <tableColumn id="2" xr3:uid="{D5FECD6D-54D4-413E-86EE-CACF52D2DA63}" name="String EN"/>
@@ -781,15 +799,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBD24C1D-54A3-4D83-9E6C-EC9C7BE97A48}">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="29.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.73046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.19921875" customWidth="1"/>
     <col min="3" max="3" width="42.19921875" customWidth="1"/>
   </cols>
@@ -1309,6 +1327,28 @@
       </c>
       <c r="C47" s="2" t="s">
         <v>123</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A48" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A49" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new localized strings
</commit_message>
<xml_diff>
--- a/loca/Loca_Keys_Strings_DE_EN.xlsx
+++ b/loca/Loca_Keys_Strings_DE_EN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\Desktop\vintage-poker\loca\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick O-Punkt\Desktop\vintage-poker\loca\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F68F21-22F5-459E-B5BE-80FD54BFCB10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E82728-238A-4F41-A9DA-FAD6C3088FB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2220" windowWidth="21600" windowHeight="11535" xr2:uid="{94609645-BEC5-4C02-AAB5-847C7763F872}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{94609645-BEC5-4C02-AAB5-847C7763F872}"/>
   </bookViews>
   <sheets>
     <sheet name="KeyValuePairs" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="199">
   <si>
     <t>Key</t>
   </si>
@@ -602,13 +602,37 @@
     <t>Keine Verbindung!</t>
   </si>
   <si>
-    <t>           </t>
-  </si>
-  <si>
     <t>Could not connect / lost connection to game server! Please try again  later!</t>
   </si>
   <si>
     <t>Verbindung zum Spieleserver konnte nicht hergestellt werden / Verbindung unterbrochen! Bitte versuchen Sie es später noch einmal!</t>
+  </si>
+  <si>
+    <t>global_get-free-chips-modal_header</t>
+  </si>
+  <si>
+    <t>global_get-free-chips-modal_content</t>
+  </si>
+  <si>
+    <t>global_get-free-chips-modal_btn-txt</t>
+  </si>
+  <si>
+    <t>Refuel  </t>
+  </si>
+  <si>
+    <t>Get Your Free Chips</t>
+  </si>
+  <si>
+    <t>Auftanken</t>
+  </si>
+  <si>
+    <t>Gratis Chips Holen</t>
+  </si>
+  <si>
+    <t>Oh nein, es scheint, als würden Ihnen die Chips ausgehen! Aber keine Sorge, hier ist eine neue Charge Chips für Sie, damit Sie weiterspielen können!</t>
+  </si>
+  <si>
+    <t>Oh noes, it seems like you're running out of chips! But don't worry, here's a fresh batch of chips for you so you can continue playing!</t>
   </si>
 </sst>
 </file>
@@ -650,18 +674,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -689,7 +710,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -985,20 +1006,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBD24C1D-54A3-4D83-9E6C-EC9C7BE97A48}">
-  <dimension ref="A1:C72"/>
+  <dimension ref="A1:C74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.19921875" customWidth="1"/>
-    <col min="3" max="3" width="42.19921875" customWidth="1"/>
+    <col min="1" max="1" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1009,7 +1030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1020,7 +1041,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1031,7 +1052,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1042,7 +1063,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1053,7 +1074,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1064,7 +1085,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1075,7 +1096,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1086,7 +1107,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1097,7 +1118,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1108,7 +1129,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1119,7 +1140,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1130,7 +1151,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
@@ -1141,7 +1162,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -1152,7 +1173,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
@@ -1163,7 +1184,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>60</v>
       </c>
@@ -1174,7 +1195,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>61</v>
       </c>
@@ -1185,7 +1206,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>62</v>
       </c>
@@ -1196,7 +1217,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>39</v>
       </c>
@@ -1207,7 +1228,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>42</v>
       </c>
@@ -1218,7 +1239,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>44</v>
       </c>
@@ -1229,7 +1250,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>43</v>
       </c>
@@ -1240,7 +1261,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>47</v>
       </c>
@@ -1251,7 +1272,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>48</v>
       </c>
@@ -1262,7 +1283,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
@@ -1273,7 +1294,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>66</v>
       </c>
@@ -1284,7 +1305,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>67</v>
       </c>
@@ -1295,7 +1316,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>71</v>
       </c>
@@ -1306,7 +1327,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>72</v>
       </c>
@@ -1317,7 +1338,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>73</v>
       </c>
@@ -1328,7 +1349,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>74</v>
       </c>
@@ -1339,7 +1360,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>82</v>
       </c>
@@ -1350,7 +1371,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>81</v>
       </c>
@@ -1361,7 +1382,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>88</v>
       </c>
@@ -1372,7 +1393,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>89</v>
       </c>
@@ -1383,7 +1404,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>94</v>
       </c>
@@ -1394,7 +1415,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>95</v>
       </c>
@@ -1405,7 +1426,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>96</v>
       </c>
@@ -1416,7 +1437,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>97</v>
       </c>
@@ -1427,7 +1448,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>98</v>
       </c>
@@ -1438,7 +1459,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>105</v>
       </c>
@@ -1449,7 +1470,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>112</v>
       </c>
@@ -1460,7 +1481,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>106</v>
       </c>
@@ -1471,7 +1492,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>107</v>
       </c>
@@ -1482,7 +1503,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>108</v>
       </c>
@@ -1493,7 +1514,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>109</v>
       </c>
@@ -1504,7 +1525,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="57" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>121</v>
       </c>
@@ -1515,7 +1536,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>124</v>
       </c>
@@ -1526,7 +1547,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>125</v>
       </c>
@@ -1537,7 +1558,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>130</v>
       </c>
@@ -1548,7 +1569,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>133</v>
       </c>
@@ -1559,7 +1580,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>134</v>
       </c>
@@ -1570,7 +1591,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>138</v>
       </c>
@@ -1581,7 +1602,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>141</v>
       </c>
@@ -1592,7 +1613,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>142</v>
       </c>
@@ -1603,7 +1624,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>143</v>
       </c>
@@ -1614,7 +1635,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>144</v>
       </c>
@@ -1625,7 +1646,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>145</v>
       </c>
@@ -1636,7 +1657,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>146</v>
       </c>
@@ -1647,7 +1668,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>157</v>
       </c>
@@ -1658,7 +1679,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>160</v>
       </c>
@@ -1669,7 +1690,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>161</v>
       </c>
@@ -1680,7 +1701,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>162</v>
       </c>
@@ -1691,7 +1712,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>163</v>
       </c>
@@ -1702,7 +1723,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>164</v>
       </c>
@@ -1713,7 +1734,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>165</v>
       </c>
@@ -1724,7 +1745,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>177</v>
       </c>
@@ -1735,7 +1756,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>182</v>
       </c>
@@ -1746,7 +1767,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>183</v>
       </c>
@@ -1757,7 +1778,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>184</v>
       </c>
@@ -1768,20 +1789,48 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>185</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="C71" s="2" t="s">
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B72" s="3" t="s">
-        <v>188</v>
+      <c r="B72" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>